<commit_message>
EPBDS-9049 one more functional test
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9049_number_as_date.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9049_number_as_date.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vpikus\.openl-webstudio\user-workspace\admin\EPBDS-9049_number_as_date\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A69BA6-ED3A-4CA3-87D5-5137282EB333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E7E035-14CC-4069-9E00-F2F5B4BF027E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="51">
   <si>
     <t>Datatype NumberAsDateType</t>
   </si>
@@ -78,12 +78,6 @@
     <t>arg1</t>
   </si>
   <si>
-    <t>DateCell</t>
-  </si>
-  <si>
-    <t>= 11/11/1900</t>
-  </si>
-  <si>
     <t>_res_.$FromData.defaultValue</t>
   </si>
   <si>
@@ -121,17 +115,79 @@
   </si>
   <si>
     <t>11/11/1900</t>
+  </si>
+  <si>
+    <t>Rules String someRule(Date myDate)</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>myDate == dateAsDouble</t>
+  </si>
+  <si>
+    <t>Cond</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>= error("Ooops")</t>
+  </si>
+  <si>
+    <t>RET1</t>
+  </si>
+  <si>
+    <t>Res</t>
+  </si>
+  <si>
+    <t>String s</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Date dateAsDouble</t>
+  </si>
+  <si>
+    <t>Test someRule</t>
+  </si>
+  <si>
+    <t>myDate</t>
+  </si>
+  <si>
+    <t>_res_</t>
+  </si>
+  <si>
+    <t>_error_</t>
+  </si>
+  <si>
+    <t>Ooops</t>
+  </si>
+  <si>
+    <t>SimpleRules String someSimpleRules(Date myDate)</t>
+  </si>
+  <si>
+    <t>My Date</t>
+  </si>
+  <si>
+    <t>Test someSimpleRules</t>
+  </si>
+  <si>
+    <t>SmartRules String someSmartRules(Date myDate)</t>
+  </si>
+  <si>
+    <t>Test someSmartRules</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -155,17 +211,17 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -446,26 +502,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:J28"/>
+  <dimension ref="B3:J74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="26.44140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.33203125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.5546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="6.5546875" collapsed="true"/>
+    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.5546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -487,10 +544,10 @@
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
@@ -517,10 +574,10 @@
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -545,7 +602,7 @@
       <c r="C18">
         <v>2</v>
       </c>
-      <c r="J18" s="4"/>
+      <c r="J18" s="3"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
@@ -557,21 +614,21 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
@@ -586,65 +643,296 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="3">
+        <v>22</v>
+      </c>
+      <c r="D24" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D25" s="3">
+        <v>23</v>
+      </c>
+      <c r="D25" s="2">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="3">
+        <v>24</v>
+      </c>
+      <c r="D26" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="3">
+        <v>25</v>
+      </c>
+      <c r="D27" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
-      </c>
-      <c r="D28" s="5">
+        <v>26</v>
+      </c>
+      <c r="D28" s="4">
         <v>316</v>
       </c>
     </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B31" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="5"/>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>777</v>
+      </c>
+      <c r="C36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C37" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="2">
+        <v>777</v>
+      </c>
+      <c r="E42" s="2">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>43</v>
+      </c>
+      <c r="C43" t="s">
+        <v>43</v>
+      </c>
+      <c r="D43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" t="s">
+        <v>44</v>
+      </c>
+      <c r="E44" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B50" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50" s="5"/>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>777</v>
+      </c>
+      <c r="C52" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C53" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" s="2">
+        <v>777</v>
+      </c>
+      <c r="E57" s="2">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" t="s">
+        <v>43</v>
+      </c>
+      <c r="D58" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>44</v>
+      </c>
+      <c r="C59" t="s">
+        <v>44</v>
+      </c>
+      <c r="E59" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B65" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C65" s="5"/>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>777</v>
+      </c>
+      <c r="C67" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C68" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>42</v>
+      </c>
+      <c r="C72" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" s="2">
+        <v>777</v>
+      </c>
+      <c r="E72" s="2">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>43</v>
+      </c>
+      <c r="C73" t="s">
+        <v>43</v>
+      </c>
+      <c r="D73" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" t="s">
+        <v>44</v>
+      </c>
+      <c r="E74" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B65:C65"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B31:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>